<commit_message>
WP-08: finalize stochastic pricing integration and recalibration
</commit_message>
<xml_diff>
--- a/Proyecto LEO IOT.xlsx
+++ b/Proyecto LEO IOT.xlsx
@@ -185,7 +185,7 @@
     <t>Amortización</t>
   </si>
   <si>
-    <t>“Sculpted” para mantener DSCR ≈ 1.45 en senior</t>
+    <t>“Sculpted” para mantener DSCR ≈ 1.20 en senior</t>
   </si>
   <si>
     <t>“Sculpted” (año 5–12)</t>
@@ -2306,22 +2306,22 @@
                   <c:v>1.449999999988306</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.450000000032805</c:v>
+                  <c:v>1.200000000032805</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.449999999578838</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4500000001719371</c:v>
+                  <c:v>1.2000000001719371</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>3.1689497479413244</c:v>
@@ -2377,49 +2377,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.45</c:v>
+                  <c:v>1.20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4709,7 +4709,7 @@
         <v>166</v>
       </c>
       <c r="N3" s="35">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O3" s="36">
         <f t="shared" ref="O3:O13" si="1">C3-(D3+F3+H3)</f>
@@ -4774,7 +4774,7 @@
         <v>167</v>
       </c>
       <c r="N4" s="35">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O4" s="36">
         <f t="shared" si="1"/>
@@ -4840,7 +4840,7 @@
         <v>168</v>
       </c>
       <c r="N5" s="35">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O5" s="36">
         <f t="shared" si="1"/>
@@ -4909,7 +4909,7 @@
         <v>170</v>
       </c>
       <c r="N6" s="35">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O6" s="36">
         <f t="shared" si="1"/>
@@ -4975,7 +4975,7 @@
         <v>171</v>
       </c>
       <c r="N7" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O7" s="36">
         <f t="shared" si="1"/>
@@ -5035,7 +5035,7 @@
         <v>11.586206896551724</v>
       </c>
       <c r="K8" s="34">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>172</v>
@@ -5044,7 +5044,7 @@
         <v>173</v>
       </c>
       <c r="N8" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O8" s="36">
         <f t="shared" si="1"/>
@@ -5104,13 +5104,13 @@
         <v>14.206896551724141</v>
       </c>
       <c r="K9" s="34">
-        <v>1.450000000032805</v>
+        <v>1.200000000032805</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>174</v>
       </c>
       <c r="N9" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O9" s="36">
         <f t="shared" si="1"/>
@@ -5173,7 +5173,7 @@
         <v>1.449999999578838</v>
       </c>
       <c r="N10" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O10" s="36">
         <f t="shared" si="1"/>
@@ -5233,13 +5233,13 @@
         <v>16.27586206896552</v>
       </c>
       <c r="K11" s="34">
-        <v>1.4500000001719371</v>
+        <v>1.2000000001719371</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>175</v>
       </c>
       <c r="N11" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O11" s="36">
         <f t="shared" si="1"/>
@@ -5299,10 +5299,10 @@
         <v>14.655172413793103</v>
       </c>
       <c r="K12" s="34">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="N12" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O12" s="36">
         <f t="shared" si="1"/>
@@ -5362,13 +5362,13 @@
         <v>12.13793103448276</v>
       </c>
       <c r="K13" s="34">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>176</v>
       </c>
       <c r="N13" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O13" s="36">
         <f t="shared" si="1"/>
@@ -5432,7 +5432,7 @@
         <v>3.1689497479413244</v>
       </c>
       <c r="N14" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
@@ -5487,7 +5487,7 @@
         <v>178</v>
       </c>
       <c r="N15" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O15" s="19"/>
       <c r="P15" s="19"/>
@@ -5539,7 +5539,7 @@
         <v>179</v>
       </c>
       <c r="N16" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
@@ -5591,7 +5591,7 @@
         <v>180</v>
       </c>
       <c r="N17" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="O17" s="19"/>
       <c r="P17" s="19"/>
@@ -7726,7 +7726,7 @@
         <v>11.586206896551724</v>
       </c>
       <c r="Z7" s="53">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="AA7" s="52">
         <f>MAX(0, CFADS!I9 - Y7)</f>
@@ -7864,7 +7864,7 @@
         <v>14.206896551724137</v>
       </c>
       <c r="Z8" s="53">
-        <v>1.450000000032805</v>
+        <v>1.200000000032805</v>
       </c>
       <c r="AA8" s="52">
         <f>MAX(0, CFADS!I10 - Y8)</f>
@@ -8140,7 +8140,7 @@
         <v>16.27586206896552</v>
       </c>
       <c r="Z10" s="53">
-        <v>1.4500000001719371</v>
+        <v>1.2000000001719371</v>
       </c>
       <c r="AA10" s="52">
         <f>MAX(0, CFADS!I12 - Y10)</f>
@@ -8278,7 +8278,7 @@
         <v>14.655172413793103</v>
       </c>
       <c r="Z11" s="53">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="AA11" s="52">
         <f>MAX(0, CFADS!I13 - Y11)</f>
@@ -8416,7 +8416,7 @@
         <v>12.137931034482762</v>
       </c>
       <c r="Z12" s="53">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
       <c r="AA12" s="52">
         <f>MAX(0, CFADS!I14 - Y12)</f>
@@ -9476,7 +9476,7 @@
         <v>398</v>
       </c>
       <c r="B10" s="19">
-        <v>1.45</v>
+        <v>1.20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>